<commit_message>
Brainstorm Seguidor de Trilha
</commit_message>
<xml_diff>
--- a/Administracao/Controle/presencas_e_entregas.xlsx
+++ b/Administracao/Controle/presencas_e_entregas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Presenças" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
   <si>
     <t xml:space="preserve">Reunião – 25/07/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brainstorm – Sprint 0</t>
   </si>
   <si>
     <t xml:space="preserve">Aleff</t>
@@ -120,11 +123,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,51 +146,85 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -287,30 +325,66 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -346,6 +420,7 @@
     <dxf>
       <font>
         <name val="FreeSans"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF006600"/>
       </font>
@@ -358,6 +433,7 @@
     <dxf>
       <font>
         <name val="FreeSans"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FFCC0000"/>
       </font>
@@ -370,6 +446,7 @@
     <dxf>
       <font>
         <name val="FreeSans"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF996600"/>
       </font>
@@ -450,15 +527,16 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,7 +546,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -483,12 +563,14 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -503,12 +585,14 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -523,14 +607,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -543,12 +629,14 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -563,12 +651,14 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -583,12 +673,14 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -603,12 +695,14 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -623,12 +717,14 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -643,12 +739,14 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -663,12 +761,14 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -683,12 +783,14 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -703,12 +805,14 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -723,12 +827,14 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -743,12 +849,14 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -763,12 +871,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -783,12 +893,14 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -803,12 +915,14 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -823,12 +937,14 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -843,12 +959,14 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -863,12 +981,14 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -883,12 +1003,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -903,12 +1025,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -923,12 +1047,14 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -943,12 +1069,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -963,12 +1091,14 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -982,7 +1112,7 @@
       <c r="N26" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:M26">
+  <conditionalFormatting sqref="B2:M3 B5:M26 B4:D4 F4:M4">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Ok"</formula>
     </cfRule>
@@ -1010,14 +1140,14 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1025,7 +1155,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="n">
@@ -1061,7 +1191,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1079,7 +1209,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1097,7 +1227,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1115,7 +1245,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1133,7 +1263,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1151,7 +1281,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1169,7 +1299,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1187,7 +1317,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1205,7 +1335,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1223,7 +1353,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1241,7 +1371,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1259,7 +1389,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1277,7 +1407,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1295,7 +1425,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1313,7 +1443,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1331,7 +1461,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1349,7 +1479,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1367,7 +1497,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1385,7 +1515,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1403,7 +1533,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1421,7 +1551,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1439,7 +1569,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1457,7 +1587,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1475,7 +1605,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1493,7 +1623,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1523,7 +1653,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Organização das faltas e strikes
</commit_message>
<xml_diff>
--- a/Administracao/Controle/presencas_e_entregas.xlsx
+++ b/Administracao/Controle/presencas_e_entregas.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presenças" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Entregas" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Respostas_Entregues" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Strikes" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="37">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -32,6 +33,15 @@
     <t xml:space="preserve">Brainstorm – Sprint 0</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprint 1 – 03/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 2 – 10/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 3 – 17/08</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aleff</t>
   </si>
   <si>
@@ -68,9 +78,6 @@
     <t xml:space="preserve">Fabiano</t>
   </si>
   <si>
-    <t xml:space="preserve">Felipe Osório</t>
-  </si>
-  <si>
     <t xml:space="preserve">Filipe Freitas</t>
   </si>
   <si>
@@ -114,6 +121,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ygor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strike 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strike 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strike 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
   </si>
 </sst>
 </file>
@@ -374,7 +393,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,6 +408,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -525,10 +552,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -536,7 +563,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,9 +579,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -563,15 +599,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -585,15 +623,17 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -607,15 +647,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -629,15 +671,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -651,15 +695,17 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -673,15 +719,17 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -695,15 +743,17 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -717,15 +767,17 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -739,15 +791,17 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -761,15 +815,17 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -783,15 +839,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -805,15 +863,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -827,15 +887,17 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -849,15 +911,17 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -871,15 +935,17 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -893,15 +959,17 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -915,15 +983,17 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -937,15 +1007,17 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -959,15 +1031,17 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -981,15 +1055,17 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1003,15 +1079,17 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1025,15 +1103,17 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1047,15 +1127,17 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1069,15 +1151,17 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1089,30 +1173,8 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:M3 B5:M26 B4:D4 F4:M4">
+  <conditionalFormatting sqref="B2:M3 B5:M25 B4:D4 F4:M4">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Ok"</formula>
     </cfRule>
@@ -1138,10 +1200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1191,9 +1253,11 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1209,9 +1273,11 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1227,9 +1293,11 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1245,9 +1313,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1263,9 +1333,11 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1281,9 +1353,11 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1299,9 +1373,11 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1317,9 +1393,11 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1335,9 +1413,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1353,9 +1433,11 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1371,9 +1453,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1389,9 +1473,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1407,9 +1493,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1425,9 +1513,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1443,9 +1533,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1461,9 +1553,11 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1479,9 +1573,11 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1497,9 +1593,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1515,9 +1613,11 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1533,9 +1633,11 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1551,9 +1653,11 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1569,9 +1673,11 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1587,9 +1693,11 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1605,9 +1713,11 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1621,26 +1731,8 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:M26">
+  <conditionalFormatting sqref="B2:M25">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Ok"</formula>
     </cfRule>
@@ -1659,4 +1751,245 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D25">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Entregas na sprint 1
</commit_message>
<xml_diff>
--- a/Administracao/Controle/presencas_e_entregas.xlsx
+++ b/Administracao/Controle/presencas_e_entregas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="37">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -555,7 +555,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -564,7 +564,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -682,7 +682,9 @@
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -826,7 +828,9 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -970,7 +974,9 @@
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -994,7 +1000,9 @@
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1090,7 +1098,9 @@
       <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1114,7 +1124,9 @@
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1203,7 +1215,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1258,7 +1270,9 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1278,7 +1292,9 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1298,7 +1314,9 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1318,7 +1336,9 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1338,7 +1358,9 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1358,7 +1380,9 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1378,7 +1402,9 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1398,7 +1424,9 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1418,7 +1446,9 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1438,7 +1468,9 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1458,7 +1490,9 @@
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1478,7 +1512,9 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1498,7 +1534,9 @@
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1518,7 +1556,9 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1538,7 +1578,9 @@
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1558,7 +1600,9 @@
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1578,7 +1622,9 @@
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1598,7 +1644,9 @@
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1618,7 +1666,9 @@
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1638,7 +1688,9 @@
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1658,7 +1710,9 @@
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1678,7 +1732,9 @@
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1698,7 +1754,9 @@
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1718,7 +1776,9 @@
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>

</xml_diff>